<commit_message>
adjusted wiring sheet for motor drivers
</commit_message>
<xml_diff>
--- a/Wiring.xlsx
+++ b/Wiring.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed\Desktop\TableProj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3B2F2ED-B0F3-43CA-BC7D-C31724CC370C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB7C4C8-2CF7-4ACF-A567-1EA2E3D6A778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2985" yWindow="2985" windowWidth="18000" windowHeight="9360" xr2:uid="{E038C72C-96D2-4CED-AB3C-C0AF9D7D15E2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>D0</t>
   </si>
@@ -48,12 +48,6 @@
     <t>D10</t>
   </si>
   <si>
-    <t>driver input for actuator 1</t>
-  </si>
-  <si>
-    <t>driver input for actuator 2</t>
-  </si>
-  <si>
     <t>D12</t>
   </si>
   <si>
@@ -88,6 +82,24 @@
   </si>
   <si>
     <t>On/Off button</t>
+  </si>
+  <si>
+    <t>RPWM for actuator 1</t>
+  </si>
+  <si>
+    <t>LPWM for actuator 2</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>LPWM for actuator 1</t>
+  </si>
+  <si>
+    <t>RPWM for actuator 2</t>
   </si>
 </sst>
 </file>
@@ -439,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F44DDDFD-78CF-424A-9761-A986590A4698}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,7 +467,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -463,7 +475,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -471,7 +483,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -479,47 +491,63 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>